<commit_message>
We started cleaning the data in more detail
</commit_message>
<xml_diff>
--- a/Data_ML_filled.xlsx
+++ b/Data_ML_filled.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3917,7 +3917,7 @@
 Die in der Pflege tätigen Personen sollen entsprechend ihrer Ausbildung und ihren Kompetenzen eingesetzt werden. So soll der Bund die Arbeitsbedingungen in den Spitälern, Heimen und Spitexorganisationen verbindlich regeln. Dazu zählt die Höhe der Löhne.
 Zudem sollen Pflegefachpersonen gewisse Pflegeleistungen selbständig direkt mit der obligatorischen Krankenpflegeversicherung oder anderen Sozialversicherungen abrechnen können. Heute können sie grundsätzlich nur die Leistungen abrechnen, die von einer Ärztin oder einem Arzt angeordnet worden sind.
 Dem Bundesrat und einer Mehrheit des Parlaments geht dieser Vorschlag zu weit. Das Parlament hat deshalb einen indirekten Gegenvorschlag zur Volksinitiative verabschiedet. Dieser Vorschlag tritt in Kraft, wenn die Initiative abgelehnt wird und der Gegenvorschlag nicht erfolgreich mit einem Referendum bekämpft wird.
-Der Gegenvorschlag sieht unter anderem vor, dass Bund und Kantone für die nächsten acht Jahre rund eine Milliarde Franken in die Ausbildung von Pflegepersonal investieren. Mit dem Geld sollen sowohl Studierende als auch Spitäler, Pflegeheime und Spitexorganisationen unterstützt werden, die Pflegepersonal ausbilden.
+Der Gegenvorschlag sieht unter anderem vor, dass Bund und Kantone für die nächsten acht Jahre rund eine Milliarde Franken in die Ausbildung von Pflegepersonal investieren. Mit dem Geld sollen sowohl Studierende als auch Spitäler, Pflegeheime und Spitexorganisationen unterstützt werden, die Pflegepersonal ausbilden.
 Zudem sollen Fachhochschulen und höhere Fachschulen Geld erhalten, wenn sie die Zahl der Ausbildungsplätze erhöhen.   Für Bundesrat und Parlament geht die Pflegeinitiative zu weit. Sie unterstützen den indirekten Gegenvorschlag. Dieser sieht unter anderem vor, dass Bund und Kantone für die nächsten acht Jahre rund eine Milliarde Franken in die Ausbildung von neuem Pflegepersonal investiert. Der indirekte Gegenvorschlag sei im Gegensatz zur Initiative konkreter und auch schneller umsetzbar, so die Ansicht der Initiativ-Gegner. «Einfach die Wünsche an eine bessere Pflege in die Verfassung zu schreiben, reicht nicht», sagt beispielsweise Jörg Kündig, FDP-Kantonsrat in Zürich und Gesundheitspolitiker. Ihm fehlen die konkreten Schritte, wie das Problem gelöst wird, deshalb engagiert er sich für den Gegenvorschlag. Für die Initianten der Volksinitiative geht der Gegenvorschlag zu wenig weit. Er beinhalte wesentliche Inhalte nicht, wie zum Beispiel die Verbesserung der Arbeitsbedingungen und eine verbindliche Vorgabe, wie viele Patientinnen eine Pflegeperson maximal betreut. Bessere Arbeitsbedingungen in der Pflege: Braucht es die Initiative oder reicht der Gegenvorschlag? Am Donnerstag 28.10., ab 20 Uhr diskutierten folgende Gäste in der Sendung «Forum»: .  Radio SRF 1, Sendung «Forum», 28.10.2021, 20 Uhr Auf einen Blick Nein-Komitee Abstimmung am 28. November Für die Registrierung benötigen wir zusätzliche Angaben zu Ihrer Person. Bitte melden Sie sich an, um einen Kommentar zu erfassen. {| foundExistingAccountText |} {| current_emailAddress |}. Geben Sie die E-Mail-Adresse Ihres Benutzerkontos an. Wir senden Ihnen anschliessend einen Link, über den Sie ein neues Passwort erstellen können. abbrechen Sie erhalten in Kürze eine E-Mail mit einem Link, um Ihr Passwort zu erneuern. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM Ordner und die Angabe Ihrer E-Mail-Adresse. Bitte melden Sie sich an, um einen Kommentar zu erfassen. Oh Hoppla! Es ist ein technischer Fehler aufgetreten. Bitte versuchen Sie es später noch ein Mal oder kontaktieren Sie unseren Kundendienst. Damit Sie einen Kommentar erfassen können, bitten wir Sie, Ihre Mobilnummer zu bestätigen. Wir senden Ihnen einen SMS-Code an die Mobilnummer . Es ist ein Fehler aufgetreten. Bitte versuchen Sie es erneut oder kontaktieren Sie unseren Kundendienst. Es wurden bereits zu viele Codes für die Mobilnummer angefordert. Um Missbrauch zu verhindern, wird die Funktion blockiert. Zu viele Versuche. Bitte fordern Sie einen neuen Code an oder kontaktieren Sie unseren Kundendienst. SMS-Code anfordern Mobilnummer ändern Wir haben Ihnen einen SMS-Code an die Mobilnummer  gesendet. Bitte geben Sie den SMS-Code in das untenstehende Feld ein. Code erneut anfordern Mobilnummer ändern Zu viele Versuche. Bitte fordern Sie einen neuen Code an oder kontaktieren Sie unseren Kundendienst. Diese Mobilnummer wird bereits verwendet. Bitte ändern Sie Ihre Mobilnummer oder wenden Sie sich an unseren Kundendienst. Mobilnummer ändern Die maximale Anzahl an Codes für die angegebene Nummer ist erreicht. Es können keine weiteren Codes erstellt werden. An diese Nummer senden wir Ihnen einen Aktivierungscode. Wir haben Ihnen ein E-Mail an die Adresse {* emailAddressData *} gesendet. Prüfen Sie bitte Ihr E-Mail-Postfach und bestätigen Sie Ihren Account über den erhaltenen Aktivierungslink. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM-Ordner und die Angabe Ihrer E-Mail-Adresse. Benutzerdaten anpassen {* resendLink *} Mit einem SRF-Account erhalten Sie die Möglichkeit, Kommentare auf unserer Webseite sowie in der SRF App zu erfassen. Wir haben Ihnen ein E-Mail an die Adresse {* emailAddressData *} gesendet. Prüfen Sie bitte Ihr E-Mail-Postfach und bestätigen Sie Ihren Account über den erhaltenen Aktivierungslink. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM-Ordner und die Angabe Ihrer E-Mail-Adresse. Benutzerdaten anpassen {* resendLink *} Bitte prüfen Sie Ihr E-Mail-Postfach. Das Aktivierungs-E-Mail wurde versendet. Vielen Dank für die Verifizierung Ihrer E-Mail-Adresse. In dieser Ansicht können Sie Ihre Benutzerdaten verwalten. Passwort ändern Account deaktivieren Sie können Ihre Daten jederzeit in Ihrem Benutzerkonto einsehen. Benutzerdaten anpassen Definieren Sie ein neues Passwort für Ihren Account {* emailAddressData *}. abbrechen Definieren Sie ein neues Passwort für Ihren Account. Sie können sich nun im Artikel mit Ihrem neuen Passwort anmelden. Wir haben den Code zum Passwort neusetzen nicht erkannt. Bitte geben Sie Ihre E-Mail-Adresse erneut ein, damit wir Ihnen einen neuen Link zuschicken können. Sie erhalten in Kürze eine E-Mail mit einem Link, um Ihr Passwort zu erneuern. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM Ordner und die Angabe Ihrer E-Mail-Adresse. Ihr Account wird deaktiviert und kann von Ihnen nicht wieder aktiviert werden. Erfasste Kommentare werden nicht gelöscht. Wollen Sie Ihren Account wirklich deaktivieren? Ihr Account wurde deaktiviert und kann nicht weiter verwendet werden.
         Wenn Sie sich erneut für die Kommentarfunktion registrieren möchten, melden Sie sich bitte beim Kundendienst von SRF. SRF Schweizer Radio und Fernsehen,Zweigniederlassung der Schweizerischen Radio- und Fernsehgesellschaft</t>
         </is>
@@ -4144,7 +4144,7 @@
       <c r="J81" t="inlineStr">
         <is>
           <t>Einige Elemente auf SRF.ch funktionieren nur mit aktiviertem JavaScript. Heute werden die Richterinnen und Richter für das Bundesgericht vom Parlament gewählt. Die Justizinitiative will das ändern – und die Richter im Losverfahren bestimmen. Damit soll das Bundesgericht unabhängiger von den Parteien werden. Autor: 
-Rafael von Matt 02.11.2021, 13:41  «Wollen Sie unabhängige Richterinnen und Richter?» Diese Frage stellt die Ja-Kampagne der Justizinitiative. Hinter der Frage steht die Überzeugung des Initiativkomitees, dass die 38 Bundesrichterinnen und -richter heute nicht unabhängig, sondern abhängig von ihren Parteien sind. Tatsächlich wählt das Parlament die Richterinnen und Richter für das höchste Gericht des Landes in Lausanne. Und seit 1953 gehören alle Gewählten einer Partei an. Seit fast 70 Jahren haben Parteilose also keine Chance mehr, Bundesrichterin oder Bundesrichter zu werden. Diese Verflechtung zwischen Politik und Justiz wird regelmässig kritisiert – etwa auch vom Europarat. Hier setzt die Justizinitiative an, die der Unternehmer Adrian Gasser 2018 lancierte und über die wir am 28. November abstimmen: Die Initiative fordert, dass die Bundesrichterinnen und -richter in Zukunft im Losverfahren gewählt werden. Im «Forum» diskutieren Fachleute mit Hörerinnen und Hörern brennende aktuelle Themen aus Gesellschaft, Politik, Wirtschaft, Kultur oder Sport. Das «Forum» ist live.
+Rafael von Matt 02.11.2021, 13:41  «Wollen Sie unabhängige Richterinnen und Richter?» Diese Frage stellt die Ja-Kampagne der Justizinitiative. Hinter der Frage steht die Überzeugung des Initiativkomitees, dass die 38 Bundesrichterinnen und -richter heute nicht unabhängig, sondern abhängig von ihren Parteien sind. Tatsächlich wählt das Parlament die Richterinnen und Richter für das höchste Gericht des Landes in Lausanne. Und seit 1953 gehören alle Gewählten einer Partei an. Seit fast 70 Jahren haben Parteilose also keine Chance mehr, Bundesrichterin oder Bundesrichter zu werden. Diese Verflechtung zwischen Politik und Justiz wird regelmässig kritisiert – etwa auch vom Europarat. Hier setzt die Justizinitiative an, die der Unternehmer Adrian Gasser 2018 lancierte und über die wir am 28. November abstimmen: Die Initiative fordert, dass die Bundesrichterinnen und -richter in Zukunft im Losverfahren gewählt werden. Im «Forum» diskutieren Fachleute mit Hörerinnen und Hörern brennende aktuelle Themen aus Gesellschaft, Politik, Wirtschaft, Kultur oder Sport. Das «Forum» ist live.
 Der Hörer- und Usereinbezug ist das Markenzeichen der Sendung «Forum». Die Hörerinnen und Hörer sind entweder live im Studio oder aber sie beteiligen sich per Telefon oder an der Online-Diskussion auf srf1.ch. Eine unabhängige Expertenkommission soll jene Personen auswählen, die für die Wahl geeignet sind, bevor das Los entscheidet. Damit sollen auch Parteilose wieder eine Chance haben – und die Verflechtung mit den Parteien durchbrochen werden. Der Bundesrat und alle Parteien bekämpfen die Initiative. Sie argumentieren, es gebe keine Hinweise, dass Bundesrichterinnen und -richter nicht unabhängig urteilten. Ausserdem sei das heutige System demokratisch und transparent. Hingegen schwäche das Losverfahren die demokratische Legitimation des Bundesgerichts. Und der Zufall mache nicht die geeignetsten Personen zu Bundesrichterinnen und -richtern. Über die Justizinitiative diskutieren wir am Donnerstag, 4. November, in der Sendung «Forum». Gäste in der Sendung sind:  Radio SRF 1, Sendung «Forum», 4.11.2021, 20 Uhr Auf einen Blick Für die Registrierung benötigen wir zusätzliche Angaben zu Ihrer Person. Bitte melden Sie sich an, um einen Kommentar zu erfassen. {| foundExistingAccountText |} {| current_emailAddress |}. Geben Sie die E-Mail-Adresse Ihres Benutzerkontos an. Wir senden Ihnen anschliessend einen Link, über den Sie ein neues Passwort erstellen können. abbrechen Sie erhalten in Kürze eine E-Mail mit einem Link, um Ihr Passwort zu erneuern. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM Ordner und die Angabe Ihrer E-Mail-Adresse. Bitte melden Sie sich an, um einen Kommentar zu erfassen. Oh Hoppla! Es ist ein technischer Fehler aufgetreten. Bitte versuchen Sie es später noch ein Mal oder kontaktieren Sie unseren Kundendienst. Damit Sie einen Kommentar erfassen können, bitten wir Sie, Ihre Mobilnummer zu bestätigen. Wir senden Ihnen einen SMS-Code an die Mobilnummer . Es ist ein Fehler aufgetreten. Bitte versuchen Sie es erneut oder kontaktieren Sie unseren Kundendienst. Es wurden bereits zu viele Codes für die Mobilnummer angefordert. Um Missbrauch zu verhindern, wird die Funktion blockiert. Zu viele Versuche. Bitte fordern Sie einen neuen Code an oder kontaktieren Sie unseren Kundendienst. SMS-Code anfordern Mobilnummer ändern Wir haben Ihnen einen SMS-Code an die Mobilnummer  gesendet. Bitte geben Sie den SMS-Code in das untenstehende Feld ein. Code erneut anfordern Mobilnummer ändern Zu viele Versuche. Bitte fordern Sie einen neuen Code an oder kontaktieren Sie unseren Kundendienst. Diese Mobilnummer wird bereits verwendet. Bitte ändern Sie Ihre Mobilnummer oder wenden Sie sich an unseren Kundendienst. Mobilnummer ändern Die maximale Anzahl an Codes für die angegebene Nummer ist erreicht. Es können keine weiteren Codes erstellt werden. An diese Nummer senden wir Ihnen einen Aktivierungscode. Wir haben Ihnen ein E-Mail an die Adresse {* emailAddressData *} gesendet. Prüfen Sie bitte Ihr E-Mail-Postfach und bestätigen Sie Ihren Account über den erhaltenen Aktivierungslink. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM-Ordner und die Angabe Ihrer E-Mail-Adresse. Benutzerdaten anpassen {* resendLink *} Mit einem SRF-Account erhalten Sie die Möglichkeit, Kommentare auf unserer Webseite sowie in der SRF App zu erfassen. Wir haben Ihnen ein E-Mail an die Adresse {* emailAddressData *} gesendet. Prüfen Sie bitte Ihr E-Mail-Postfach und bestätigen Sie Ihren Account über den erhaltenen Aktivierungslink. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM-Ordner und die Angabe Ihrer E-Mail-Adresse. Benutzerdaten anpassen {* resendLink *} Bitte prüfen Sie Ihr E-Mail-Postfach. Das Aktivierungs-E-Mail wurde versendet. Vielen Dank für die Verifizierung Ihrer E-Mail-Adresse. In dieser Ansicht können Sie Ihre Benutzerdaten verwalten. Passwort ändern Account deaktivieren Sie können Ihre Daten jederzeit in Ihrem Benutzerkonto einsehen. Benutzerdaten anpassen Definieren Sie ein neues Passwort für Ihren Account {* emailAddressData *}. abbrechen Definieren Sie ein neues Passwort für Ihren Account. Sie können sich nun im Artikel mit Ihrem neuen Passwort anmelden. Wir haben den Code zum Passwort neusetzen nicht erkannt. Bitte geben Sie Ihre E-Mail-Adresse erneut ein, damit wir Ihnen einen neuen Link zuschicken können. Sie erhalten in Kürze eine E-Mail mit einem Link, um Ihr Passwort zu erneuern. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM Ordner und die Angabe Ihrer E-Mail-Adresse. Ihr Account wird deaktiviert und kann von Ihnen nicht wieder aktiviert werden. Erfasste Kommentare werden nicht gelöscht. Wollen Sie Ihren Account wirklich deaktivieren? Ihr Account wurde deaktiviert und kann nicht weiter verwendet werden.
         Wenn Sie sich erneut für die Kommentarfunktion registrieren möchten, melden Sie sich bitte beim Kundendienst von SRF. SRF Schweizer Radio und Fernsehen,Zweigniederlassung der Schweizerischen Radio- und Fernsehgesellschaft</t>
         </is>
@@ -4337,7 +4337,7 @@
         <is>
           <t>Einige Elemente auf SRF.ch funktionieren nur mit aktiviertem JavaScript. Im Februar wird über die Initiative über das Verbot von Tierversuchen abgestimmt. Sind Tierversuche unverzichtbar oder unnütze Quälerei? Autor: 
 Yvonne Hafner 18.01.2022, 15:29 Liebe Userinnen und User, die geplante «Forum»-Sendung vom Donnerstag, 20. Januar zur Tierversuchsverbotsinitiative findet aufgrund eines Ausfalls im Team von Radio SRF 1 nicht statt. Wir schliessen deshalb die Kommentare zu diesem Artikel. Danke fürs Verständnis und merci fürs Mitkommentieren!   Am 13. Februar 2022 entscheidet die Schweizer Stimmbevölkerung über die Initiative «Ja zum Tier- und Menschenversuchsverbot – Ja zu Forschungswegen mit Impulsen für Sicherheit und Fortschritt», kurz Tierversuchsverbots-Initiative. Wer mit Tieren forscht, wird dem Tier in vielen Fällen Schaden zufügen: Es wird verletzt, krank gemacht und psychischem Stress ausgesetzt. Deshalb fordert die Initiative ein bedingungsloses Verbot von Tierversuchen. Zudem soll der Import von Produkten und Medikamenten, die mit Tierversuchen entwickelt wurden, verboten werden. Auch klinische Studien noch nicht zugelassener Medikamente an gesunden Menschen, von den Initiantinnen «Menschenversuche» genannt, würden bei Annahme der Initiative verboten. «Die Menschenversuche liefern nur vage Durchschnittswerte», sagt Regina Möckli vom Unterstützungskomitee. Die Initianten argumentieren zudem, Tierversuche seien ineffizient: Die Körper von Tieren unterschieden sich zu stark von jenen der Menschen. Von 100 Wirkstoffen versagten 95 im Menschenversuch, trotz scheinbar erfolgversprechender Ergebnisse im Tierversuch. Lanciert wurde die Initiative von der Interessengemeinschaft Tierversuchsverbot Schweiz – einer kleinen Gruppe von Tierschützerinnen und Tierschützern ohne politische Bindung.
-Bundesrat und Parlament lehnen die Initiative geschlossen ab. Auch viele Verbände und Interessegruppen sind dagegen: zum Beispiel Economiesuisse, die Ärztevereinigung FMH, der Schweizer Tierschutz und der Schweizerische Nationalfonds. Für die Initiative findet sich weder bei Parteien und noch bei Verbänden Unterstützung – zumindest offiziell.  Fakt ist: Rund 600'000 Tiere pro Jahr werden in der Schweiz in Tierversuchen von Universitäten, Spitälern oder Pharma eingesetzt – Fische, Mäuse, Vögel, Katzen, Hunde oder Affen. Knapp ein Drittel davon müssen belastende Experimente über sich ergehen lassen. Die schwersten Versuche des «Schweregrades 3» sind mit starken Schmerzen oder Angst, schweren Beeinträchtigungen und langfristigen Leiden verbunden. Während in den letzten Jahren die Anzahl der Tierversuche stark abgenommen hat, nehmen die besonders belastenden Versuche nach wie vor zu. Forscherinnen und Forscher bezeichnen die Initiative aber als radikal: Ganz ohne Einsatz von Tieren sei im Moment wissenschaftlicher Fortschritt nicht möglich. Mit dem Importverbot für Medikamente, die mit Tierversuchen hergestellt wurden, würde sich die Schweiz ins Mittelalter zurückkatapultieren.  Bei einer Annahme gäbe es in der Schweiz keine neuen Medikamente, Therapien oder Impfstoffe mehr, weder für Menschen noch für Tiere. «Wir hätten keine Impfungen und kein einziges Antibiotikum mehr. Und auch keine Medikamente gegen schwere Krankheiten wie Krebs», befürchtet beispielsweise der Tierforscher Robert Rieben von der Uni Bern. Die Schweiz habe im internationalen Vergleich bereits eines der strengsten Tierschutzgesetze, argumentieren die Initiativ-Gegner. Tierversuche dürfen nur dann durchgeführt werden, wenn keine Alternativen zur Verfügung stehen. Zudem muss jeder Versuch vom kantonalen Veterinäramt und der jeweiligen Tierversuchskommission bewilligt werden. Würde die Initiative angenommen, wäre die Schweiz das erste Land, das komplett auf Tierversuche verzichtet. Im «Forum» diskutieren Fachleute mit Hörerinnen und Hörern brennende aktuelle Themen aus Gesellschaft, Politik, Wirtschaft, Kultur oder Sport. Das «Forum» ist live.
+Bundesrat und Parlament lehnen die Initiative geschlossen ab. Auch viele Verbände und Interessegruppen sind dagegen: zum Beispiel Economiesuisse, die Ärztevereinigung FMH, der Schweizer Tierschutz und der Schweizerische Nationalfonds. Für die Initiative findet sich weder bei Parteien und noch bei Verbänden Unterstützung – zumindest offiziell.  Fakt ist: Rund 600'000 Tiere pro Jahr werden in der Schweiz in Tierversuchen von Universitäten, Spitälern oder Pharma eingesetzt – Fische, Mäuse, Vögel, Katzen, Hunde oder Affen. Knapp ein Drittel davon müssen belastende Experimente über sich ergehen lassen. Die schwersten Versuche des «Schweregrades 3» sind mit starken Schmerzen oder Angst, schweren Beeinträchtigungen und langfristigen Leiden verbunden. Während in den letzten Jahren die Anzahl der Tierversuche stark abgenommen hat, nehmen die besonders belastenden Versuche nach wie vor zu. Forscherinnen und Forscher bezeichnen die Initiative aber als radikal: Ganz ohne Einsatz von Tieren sei im Moment wissenschaftlicher Fortschritt nicht möglich. Mit dem Importverbot für Medikamente, die mit Tierversuchen hergestellt wurden, würde sich die Schweiz ins Mittelalter zurückkatapultieren.  Bei einer Annahme gäbe es in der Schweiz keine neuen Medikamente, Therapien oder Impfstoffe mehr, weder für Menschen noch für Tiere. «Wir hätten keine Impfungen und kein einziges Antibiotikum mehr. Und auch keine Medikamente gegen schwere Krankheiten wie Krebs», befürchtet beispielsweise der Tierforscher Robert Rieben von der Uni Bern. Die Schweiz habe im internationalen Vergleich bereits eines der strengsten Tierschutzgesetze, argumentieren die Initiativ-Gegner. Tierversuche dürfen nur dann durchgeführt werden, wenn keine Alternativen zur Verfügung stehen. Zudem muss jeder Versuch vom kantonalen Veterinäramt und der jeweiligen Tierversuchskommission bewilligt werden. Würde die Initiative angenommen, wäre die Schweiz das erste Land, das komplett auf Tierversuche verzichtet. Im «Forum» diskutieren Fachleute mit Hörerinnen und Hörern brennende aktuelle Themen aus Gesellschaft, Politik, Wirtschaft, Kultur oder Sport. Das «Forum» ist live.
 Der Hörer- und Usereinbezug ist das Markenzeichen der Sendung «Forum». Die Hörerinnen und Hörer sind entweder live im Studio oder aber sie beteiligen sich per Telefon oder an der Online-Diskussion auf srf1.ch.  Für die Registrierung benötigen wir zusätzliche Angaben zu Ihrer Person. Bitte melden Sie sich an, um einen Kommentar zu erfassen. {| foundExistingAccountText |} {| current_emailAddress |}. Geben Sie die E-Mail-Adresse Ihres Benutzerkontos an. Wir senden Ihnen anschliessend einen Link, über den Sie ein neues Passwort erstellen können. abbrechen Sie erhalten in Kürze eine E-Mail mit einem Link, um Ihr Passwort zu erneuern. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM Ordner und die Angabe Ihrer E-Mail-Adresse. Bitte melden Sie sich an, um einen Kommentar zu erfassen. Oh Hoppla! Es ist ein technischer Fehler aufgetreten. Bitte versuchen Sie es später noch ein Mal oder kontaktieren Sie unseren Kundendienst. Damit Sie einen Kommentar erfassen können, bitten wir Sie, Ihre Mobilnummer zu bestätigen. Wir senden Ihnen einen SMS-Code an die Mobilnummer . Es ist ein Fehler aufgetreten. Bitte versuchen Sie es erneut oder kontaktieren Sie unseren Kundendienst. Es wurden bereits zu viele Codes für die Mobilnummer angefordert. Um Missbrauch zu verhindern, wird die Funktion blockiert. Zu viele Versuche. Bitte fordern Sie einen neuen Code an oder kontaktieren Sie unseren Kundendienst. SMS-Code anfordern Mobilnummer ändern Wir haben Ihnen einen SMS-Code an die Mobilnummer  gesendet. Bitte geben Sie den SMS-Code in das untenstehende Feld ein. Code erneut anfordern Mobilnummer ändern Zu viele Versuche. Bitte fordern Sie einen neuen Code an oder kontaktieren Sie unseren Kundendienst. Diese Mobilnummer wird bereits verwendet. Bitte ändern Sie Ihre Mobilnummer oder wenden Sie sich an unseren Kundendienst. Mobilnummer ändern Die maximale Anzahl an Codes für die angegebene Nummer ist erreicht. Es können keine weiteren Codes erstellt werden. An diese Nummer senden wir Ihnen einen Aktivierungscode. Wir haben Ihnen ein E-Mail an die Adresse {* emailAddressData *} gesendet. Prüfen Sie bitte Ihr E-Mail-Postfach und bestätigen Sie Ihren Account über den erhaltenen Aktivierungslink. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM-Ordner und die Angabe Ihrer E-Mail-Adresse. Benutzerdaten anpassen {* resendLink *} Mit einem SRF-Account erhalten Sie die Möglichkeit, Kommentare auf unserer Webseite sowie in der SRF App zu erfassen. Wir haben Ihnen ein E-Mail an die Adresse {* emailAddressData *} gesendet. Prüfen Sie bitte Ihr E-Mail-Postfach und bestätigen Sie Ihren Account über den erhaltenen Aktivierungslink. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM-Ordner und die Angabe Ihrer E-Mail-Adresse. Benutzerdaten anpassen {* resendLink *} Bitte prüfen Sie Ihr E-Mail-Postfach. Das Aktivierungs-E-Mail wurde versendet. Vielen Dank für die Verifizierung Ihrer E-Mail-Adresse. In dieser Ansicht können Sie Ihre Benutzerdaten verwalten. Passwort ändern Account deaktivieren Sie können Ihre Daten jederzeit in Ihrem Benutzerkonto einsehen. Benutzerdaten anpassen Definieren Sie ein neues Passwort für Ihren Account {* emailAddressData *}. abbrechen Definieren Sie ein neues Passwort für Ihren Account. Sie können sich nun im Artikel mit Ihrem neuen Passwort anmelden. Wir haben den Code zum Passwort neusetzen nicht erkannt. Bitte geben Sie Ihre E-Mail-Adresse erneut ein, damit wir Ihnen einen neuen Link zuschicken können. Sie erhalten in Kürze eine E-Mail mit einem Link, um Ihr Passwort zu erneuern. Wenn Sie nach 10 Minuten kein E-Mail erhalten haben, prüfen Sie bitte Ihren SPAM Ordner und die Angabe Ihrer E-Mail-Adresse. Ihr Account wird deaktiviert und kann von Ihnen nicht wieder aktiviert werden. Erfasste Kommentare werden nicht gelöscht. Wollen Sie Ihren Account wirklich deaktivieren? Ihr Account wurde deaktiviert und kann nicht weiter verwendet werden.
         Wenn Sie sich erneut für die Kommentarfunktion registrieren möchten, melden Sie sich bitte beim Kundendienst von SRF. SRF Schweizer Radio und Fernsehen,Zweigniederlassung der Schweizerischen Radio- und Fernsehgesellschaft</t>
         </is>

</xml_diff>